<commit_message>
[TimesheetCalculatorV2] added more check in parsing date, start_time, end_time. added more tests and testdata.
</commit_message>
<xml_diff>
--- a/python_source/Timesheet_Calculator_v2/test/parser/testdata/test_parse_testdata_001.xlsx
+++ b/python_source/Timesheet_Calculator_v2/test/parser/testdata/test_parse_testdata_001.xlsx
@@ -103,9 +103,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\/mmm\/yyyy"/>
+    <numFmt numFmtId="165" formatCode="d/mmm/yyyy"/>
     <numFmt numFmtId="166" formatCode="hh:mm\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="d\/mmm\/yyyy"/>
+    <numFmt numFmtId="167" formatCode="d/mmm/yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -293,11 +293,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,7 +381,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>